<commit_message>
collective mind with lab6 and task 4.3 for barter
</commit_message>
<xml_diff>
--- a/Результаты фракталов.xlsx
+++ b/Результаты фракталов.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mir10\OneDrive\Рабочий стол\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VvIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47009944-92C0-46A9-8AD1-EE6C2541BEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DF70C1-FECA-43CC-A552-62F291588147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5568" yWindow="1164" windowWidth="16584" windowHeight="10752" xr2:uid="{31F18125-4821-4D4D-A142-7915DB592CB8}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{31F18125-4821-4D4D-A142-7915DB592CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -43,20 +43,20 @@
     <t>Кривая Серпинского</t>
   </si>
   <si>
-    <t>Солфетка Серпинского</t>
-  </si>
-  <si>
     <t>Ковёр Серпинского</t>
   </si>
   <si>
     <t>Дерево Пифагора</t>
+  </si>
+  <si>
+    <t>Салфетка Серпинского</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +64,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFCFCFA"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -224,25 +217,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -563,7 +555,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,51 +570,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="20"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.15376610000384899</v>
       </c>
       <c r="C2" s="2">
         <v>0.17404829999577401</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>0.16305999999894899</v>
       </c>
       <c r="E2" s="2">
         <v>0.181571199995232</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>0.16916360000323</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>0.175780500001565</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
       <c r="B3" s="2">
@@ -640,7 +632,7 @@
       <c r="F3" s="2">
         <v>0.23926670000219</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>0.18685069999628401</v>
       </c>
     </row>
@@ -648,27 +640,27 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>0.18679879999399401</v>
       </c>
       <c r="C4" s="2">
         <v>0.20690829999512</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>0.32812399999966102</v>
       </c>
       <c r="E4" s="2">
         <v>0.24998599999526</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>1.24495569999999</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>0.21871450000617099</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+      <c r="A5" s="17">
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -686,7 +678,7 @@
       <c r="F5" s="2">
         <v>21.677243900005099</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>0.21309720000135701</v>
       </c>
     </row>
@@ -694,27 +686,27 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>0.59399560000019802</v>
       </c>
       <c r="C6" s="2">
         <v>0.63267510000150595</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>2.92856639999808</v>
       </c>
       <c r="E6" s="2">
         <v>0.86438200000702603</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>333.38627509999702</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>0.265243900001223</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="17">
         <v>5</v>
       </c>
       <c r="B7" s="2">
@@ -729,8 +721,8 @@
       <c r="E7" s="4">
         <v>2.3542576999970999</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="7">
+      <c r="F7" s="9"/>
+      <c r="G7" s="6">
         <v>0.33609389999764899</v>
       </c>
     </row>
@@ -738,25 +730,25 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>3.6923743999941498</v>
       </c>
       <c r="C8" s="2">
         <v>12.923489100001399</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>46.622074399994702</v>
       </c>
       <c r="E8" s="2">
         <v>6.9457412000046999</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14">
+      <c r="F8" s="12"/>
+      <c r="G8" s="13">
         <v>0.86164109999663197</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+      <c r="A9" s="18">
         <v>7</v>
       </c>
       <c r="B9" s="3">
@@ -765,12 +757,12 @@
       <c r="C9" s="5">
         <v>55.7272336000023</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="6">
+      <c r="D9" s="8"/>
+      <c r="E9" s="5">
         <v>22.728476500000301</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="8">
+      <c r="F9" s="10"/>
+      <c r="G9" s="7">
         <v>0.88533250000182295</v>
       </c>
     </row>

</xml_diff>